<commit_message>
Resolvi o bug de não adicionar corretamente o de Portugues
</commit_message>
<xml_diff>
--- a/book/horario/Horario.xlsx
+++ b/book/horario/Horario.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="B"/>
@@ -53,7 +53,7 @@
     <t>QUIMICA</t>
   </si>
   <si>
-    <t>LINGUA PORTUGUESA</t>
+    <t>PORTUGUES</t>
   </si>
   <si>
     <t>LITERATURA</t>
@@ -65,7 +65,7 @@
     <t>FISICA</t>
   </si>
   <si>
-    <t>EDUCACAO FISICA</t>
+    <t>ED</t>
   </si>
   <si>
     <t>PRODUCAO</t>
@@ -77,7 +77,7 @@
     <t>BIOLOGIA</t>
   </si>
   <si>
-    <t>ARTE</t>
+    <t>ARTES</t>
   </si>
   <si>
     <t>SOCIOLOGIA</t>
@@ -94,7 +94,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,7 +104,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -117,12 +117,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -162,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -186,9 +180,6 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -495,7 +486,7 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -510,7 +501,7 @@
     <col min="9" max="9" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,9 +533,9 @@
         <v>6</v>
       </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="4" t="s">
@@ -707,7 +698,7 @@
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="9"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
@@ -738,7 +729,7 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>